<commit_message>
DP - create_forecast_ad_hoc - try to fix
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/create_forecast_basic_ad_hoc/current/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/create_forecast_basic_ad_hoc/current/inputs_outputs.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
@@ -528,7 +528,7 @@
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
+          <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B5" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.5" customHeight="1" s="5">
@@ -550,7 +550,7 @@
       </c>
       <c r="B6" s="6" t="inlineStr">
         <is>
-          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current\background_files\TAZ_V4_230518_Published.shp</t>
+          <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels\shp\TAZ_V4_240627_with_geo_info.shp</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
GK: changed input_output files in ad hoc and current,txt file folder loction, and fix small prob in pivot
</commit_message>
<xml_diff>
--- a/create_forecast_ad_hoc/create_forecast_basic_ad_hoc/current/inputs_outputs.xlsx
+++ b/create_forecast_ad_hoc/create_forecast_basic_ad_hoc/current/inputs_outputs.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -19,7 +18,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -29,26 +28,7 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="177"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="177"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="177"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <charset val="1"/>
-      <family val="0"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
@@ -70,48 +50,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -468,96 +420,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.40234375" defaultRowHeight="13.5" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.3984375" defaultRowHeight="13.8"/>
   <cols>
-    <col width="24.4" customWidth="1" style="4" min="1" max="1"/>
-    <col width="51.6" customWidth="1" style="4" min="2" max="2"/>
+    <col width="24.3984375" customWidth="1" min="1" max="1"/>
+    <col width="51.59765625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="5">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1" ht="14.25" customHeight="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t>discription</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>location</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1" s="5">
-      <c r="A2" s="6" t="inlineStr">
+    <row r="2" ht="14.25" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>מיקום תוכנת תחזית בסיס</t>
         </is>
       </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\forecast_git\create_forecast_basic\current</t>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\Tools\forecast_git\create_forecast_basic\current</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="13.5" customHeight="1" s="5">
-      <c r="A3" s="4" t="inlineStr">
+    <row r="3" ht="13.5" customHeight="1">
+      <c r="A3" t="inlineStr">
         <is>
           <t>מיקום פלט לפי גירסא</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\forecast_by_version\V4\BASE_YEAR</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>W:\Data\Forecast\forecast_by_version\V4\BASE_YEAR</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="13.5" customHeight="1" s="5">
-      <c r="A4" s="4" t="inlineStr">
+    <row r="4" ht="13.5" customHeight="1">
+      <c r="A4" t="inlineStr">
         <is>
           <t>מיקום פלט</t>
         </is>
       </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels</t>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>W:\Projects\תכניות מרחביות\דרום_מערב_122\קבצי עבודה\תחזיות_דמוגרפיות\For_approval\Reference_tabels</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1" s="5">
-      <c r="A5" s="4" t="inlineStr">
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" t="inlineStr">
         <is>
           <t>שכבה חדשה</t>
         </is>
       </c>
-      <c r="B5" s="7" t="b">
+      <c r="B5" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" ht="13.5" customHeight="1" s="5">
-      <c r="A6" s="4" t="inlineStr">
+    <row r="6" ht="13.5" customHeight="1">
+      <c r="A6" t="inlineStr">
         <is>
           <t>מיקום שכבה חדשה</t>
         </is>
       </c>
-      <c r="B6" s="6" t="inlineStr">
-        <is>
-          <t>C:\Users\dpere\Documents\JTMT\Projects\תחזיות_דמוגרפיות\קבצי עבודה\142_מתחם_אנגל\בהת\For_approval\Reference_tabels\shp\TAZ_V4_240627_with_geo_info.shp</t>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>W:\Projects\תכניות מרחביות\דרום_מערב_122\קבצי עבודה\תחזיות_דמוגרפיות\For_approval\Reference_tabels\shp\TAZ_V4_241216_with_geo_info.shp</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="13.5" customHeight="1" s="5"/>
+    <row r="10" ht="13.5" customHeight="1"/>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>